<commit_message>
rebuilding site Sun 27 Sep 2020 03:40:26 PM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/tensionData.xlsx
+++ b/engineering/courses/mae101/docs/tensionData.xlsx
@@ -111,10 +111,10 @@
     <t xml:space="preserve">Weight hanger is 0.465 lb</t>
   </si>
   <si>
-    <t xml:space="preserve">Case 1 : Test specimens of rubber: 18 inches -- 1/4 diameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case 1 : Test specimens of rubber: 12 inches -- 5/8 diameters</t>
+    <t xml:space="preserve">Case 2 : Test specimens of rubber: 18 inches -- 1/4 diameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case 3 : Test specimens of rubber: 12 inches -- 5/8 diameters</t>
   </si>
   <si>
     <t xml:space="preserve">Tension Test Raw Data II</t>
@@ -127,11 +127,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,12 +154,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="19"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -180,39 +183,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="19"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -284,7 +261,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,27 +314,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -365,7 +322,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,10 +406,10 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="I54" activeCellId="0" sqref="I54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.96"/>
@@ -772,9 +729,9 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13"/>
+      <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="2"/>
@@ -787,7 +744,7 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13"/>
+      <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -800,22 +757,22 @@
       <c r="K35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="17" t="s">
+      <c r="A38" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="2"/>
@@ -824,264 +781,264 @@
       <c r="K38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="B39" s="17" t="n">
+      <c r="A39" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B39" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="C39" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D39" s="17" t="n">
+      <c r="C39" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D39" s="7" t="n">
         <v>0.25</v>
       </c>
-      <c r="H39" s="18"/>
+      <c r="H39" s="13"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B40" s="17" t="n">
+      <c r="A40" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B40" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="C40" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D40" s="17" t="n">
+      <c r="C40" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D40" s="7" t="n">
         <v>0.25</v>
       </c>
-      <c r="H40" s="18"/>
+      <c r="H40" s="13"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="B41" s="17" t="n">
+      <c r="A41" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" s="7" t="n">
         <v>14.5</v>
       </c>
-      <c r="C41" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D41" s="17" t="n">
+      <c r="C41" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D41" s="7" t="n">
         <v>0.25</v>
       </c>
-      <c r="H41" s="19"/>
+      <c r="H41" s="14"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="B42" s="17" t="n">
+      <c r="A42" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B42" s="7" t="n">
         <v>15.5</v>
       </c>
-      <c r="C42" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D42" s="17" t="n">
+      <c r="C42" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D42" s="7" t="n">
         <v>0.25</v>
       </c>
-      <c r="H42" s="18"/>
+      <c r="H42" s="13"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="16" t="n">
+      <c r="A43" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B43" s="17" t="n">
+      <c r="B43" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="C43" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D43" s="17" t="n">
+      <c r="C43" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D43" s="7" t="n">
         <v>0.25</v>
       </c>
-      <c r="H43" s="18"/>
+      <c r="H43" s="13"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="18"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
       <c r="K44" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="17" t="s">
+      <c r="A49" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="B50" s="17" t="n">
+      <c r="A50" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B50" s="7" t="n">
         <v>24.9</v>
       </c>
-      <c r="C50" s="17" t="n">
+      <c r="C50" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="D50" s="17" t="n">
+      <c r="D50" s="7" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B51" s="17" t="n">
+      <c r="A51" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B51" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="C51" s="17" t="n">
+      <c r="C51" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="D51" s="17" t="n">
+      <c r="D51" s="7" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="B52" s="17" t="n">
+      <c r="A52" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B52" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="C52" s="17" t="n">
+      <c r="C52" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="D52" s="17" t="n">
+      <c r="D52" s="7" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="B53" s="17" t="n">
+      <c r="A53" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B53" s="7" t="n">
         <v>45</v>
       </c>
-      <c r="C53" s="17" t="n">
+      <c r="C53" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="D53" s="17" t="n">
+      <c r="D53" s="7" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B56" s="5"/>
     </row>
     <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" s="17" t="s">
+      <c r="A58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D58" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="B59" s="17" t="n">
-        <v>11.9</v>
-      </c>
-      <c r="C59" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D59" s="17" t="n">
+      <c r="A59" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B59" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="C59" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D59" s="7" t="n">
         <v>0.625</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B60" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="C60" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D60" s="17" t="n">
+      <c r="A60" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B60" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="C60" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D60" s="7" t="n">
         <v>0.625</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="B61" s="17" t="n">
+      <c r="A61" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B61" s="7" t="n">
         <v>12.2</v>
       </c>
-      <c r="C61" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D61" s="17" t="n">
+      <c r="C61" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D61" s="7" t="n">
         <v>0.625</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="B62" s="17" t="n">
+      <c r="A62" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B62" s="7" t="n">
         <v>14.4</v>
       </c>
-      <c r="C62" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D62" s="17" t="n">
+      <c r="C62" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D62" s="7" t="n">
         <v>0.625</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16" t="n">
+      <c r="A63" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B63" s="17" t="n">
+      <c r="B63" s="7" t="n">
         <v>12.5</v>
       </c>
-      <c r="C63" s="17" t="n">
-        <v>12</v>
-      </c>
-      <c r="D63" s="17" t="n">
+      <c r="C63" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D63" s="7" t="n">
         <v>0.625</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rebuilding site Sun 27 Sep 2020 03:43:16 PM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/tensionData.xlsx
+++ b/engineering/courses/mae101/docs/tensionData.xlsx
@@ -405,11 +405,11 @@
   </sheetPr>
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I54" activeCellId="0" sqref="I54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.96"/>

</xml_diff>

<commit_message>
rebuilding site Sun 27 Sep 2020 05:53:31 PM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/tensionData.xlsx
+++ b/engineering/courses/mae101/docs/tensionData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t xml:space="preserve">Tension Test Raw Data I</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tension Test Raw Data II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I54" activeCellId="0" sqref="I54"/>
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.96"/>
@@ -775,7 +778,9 @@
       <c r="D38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H38" s="2"/>
+      <c r="H38" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -1033,7 +1038,7 @@
         <v>6</v>
       </c>
       <c r="B63" s="7" t="n">
-        <v>12.5</v>
+        <v>14.5</v>
       </c>
       <c r="C63" s="7" t="n">
         <v>12</v>

</xml_diff>

<commit_message>
rebuilding site Mon 28 Sep 2020 12:27:51 AM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/tensionData.xlsx
+++ b/engineering/courses/mae101/docs/tensionData.xlsx
@@ -408,11 +408,11 @@
   </sheetPr>
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E50" activeCellId="0" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.96"/>
@@ -957,6 +957,20 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B54" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="C54" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="D54" s="7" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
         <v>17</v>

</xml_diff>